<commit_message>
Update Matrice di tracciabilità.xlsx
</commit_message>
<xml_diff>
--- a/Matrice di tracciabilità/Matrice di tracciabilità.xlsx
+++ b/Matrice di tracciabilità/Matrice di tracciabilità.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FonsYs\Desktop\Ingegneria Del Software\dodo.net\NC_05\Matrice di tracciabilità\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD mass storage\GitHubDesktop\NC_05\Matrice di tracciabilità\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3865BD6-09F2-4D63-AC71-442058D81F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BF555D-0621-41A7-9468-0027128E77F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t>Rimozione prodotti</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>N=non implementato</t>
   </si>
   <si>
@@ -274,13 +271,16 @@
   </si>
   <si>
     <t>TC_16.16</t>
+  </si>
+  <si>
+    <t>Im</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,13 +312,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -451,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -512,7 +505,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -802,24 +794,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" customWidth="1"/>
     <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="34.85546875" customWidth="1"/>
-    <col min="10" max="10" width="31.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
     <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -847,10 +840,10 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>72</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>73</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
@@ -868,10 +861,10 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -978,13 +971,13 @@
         <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>21</v>
@@ -999,13 +992,13 @@
         <v>30</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="N7" s="26" t="s">
-        <v>17</v>
+        <v>79</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="O7" s="5"/>
     </row>
@@ -1021,13 +1014,13 @@
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>25</v>
@@ -1042,13 +1035,13 @@
         <v>24</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="O8" s="5"/>
     </row>
@@ -1064,7 +1057,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>17</v>
@@ -1082,10 +1075,10 @@
         <v>17</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>17</v>
@@ -1107,7 +1100,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>17</v>
@@ -1122,13 +1115,13 @@
         <v>17</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>17</v>
@@ -1150,7 +1143,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>17</v>
@@ -1168,10 +1161,10 @@
         <v>17</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>17</v>
@@ -1184,7 +1177,7 @@
     <row r="12" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>41</v>
@@ -1193,13 +1186,13 @@
         <v>16</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>32</v>
@@ -1208,13 +1201,13 @@
         <v>17</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>17</v>
@@ -1227,7 +1220,7 @@
     <row r="13" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>42</v>
@@ -1236,7 +1229,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>17</v>
@@ -1254,10 +1247,10 @@
         <v>26</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>17</v>
@@ -1270,22 +1263,22 @@
     <row r="14" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>29</v>
@@ -1294,13 +1287,13 @@
         <v>22</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M14" s="16" t="s">
         <v>17</v>
@@ -1313,25 +1306,25 @@
     <row r="15" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>28</v>
@@ -1340,23 +1333,23 @@
         <v>23</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="O15" s="5"/>
     </row>
     <row r="16" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>43</v>
@@ -1365,7 +1358,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>17</v>
@@ -1374,7 +1367,7 @@
         <v>17</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>17</v>
@@ -1383,10 +1376,10 @@
         <v>23</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>17</v>
@@ -1434,7 +1427,7 @@
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
@@ -1453,7 +1446,7 @@
       <c r="A20" s="12"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>

</xml_diff>